<commit_message>
coms 뒤에 token.Null인식 추가
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{82CC8FD9-5505-4E6D-B56F-677D86BC4E3F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9AD71CED-D80B-4952-976A-A1A2FEDD8FC9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="17460" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A28:M50"/>
+  <oleSize ref="A40:J54"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
   <si>
     <t>int</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -140,14 +140,6 @@
   </si>
   <si>
     <t>root</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>a+b</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>a+b+c</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -265,6 +257,10 @@
   <si>
     <t>'c'</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a+1+2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -821,7 +817,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
@@ -844,10 +842,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G1" s="3"/>
     </row>
@@ -871,16 +869,16 @@
         <v>6</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H3" s="28" t="s">
         <v>25</v>
@@ -901,7 +899,7 @@
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A6" s="26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
@@ -934,7 +932,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>8</v>
@@ -951,7 +949,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="25"/>
       <c r="F11" s="5"/>
@@ -968,13 +966,13 @@
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A13" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -989,7 +987,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1013,10 +1011,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G16" s="5"/>
     </row>
@@ -1050,7 +1048,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D21" s="7">
         <v>1</v>
@@ -1082,7 +1080,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1247,16 +1245,16 @@
     </row>
     <row r="38" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A38" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>5</v>
@@ -1266,22 +1264,22 @@
     </row>
     <row r="39" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A39" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>41</v>
       </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A40" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>4</v>
@@ -1293,10 +1291,10 @@
         <v>6</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
@@ -1308,12 +1306,12 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:10" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="42" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A42" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="15"/>
@@ -1326,18 +1324,17 @@
         <v>22</v>
       </c>
       <c r="B43" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="D43" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A44" s="10"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A44" s="1"/>
       <c r="B44" s="12"/>
       <c r="C44" s="13"/>
       <c r="F44" s="5"/>
@@ -1357,7 +1354,7 @@
         <v>5</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -1390,9 +1387,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
-      <c r="A48" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="A48" s="10"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -1440,12 +1435,12 @@
         <v>9</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="1:10" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="52" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A52" s="5"/>
       <c r="B52" s="19" t="s">
         <v>25</v>
@@ -1454,7 +1449,7 @@
         <v>9</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="E52" s="10" t="s">
         <v>27</v>
@@ -1463,9 +1458,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="2" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A53" s="1"/>
-    </row>
+    <row r="53" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6"/>
     <row r="54" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6"/>
     <row r="55" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6"/>
     <row r="56" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.6"/>

</xml_diff>